<commit_message>
COMMIT file tổng hợp tài liệu cần nộp
</commit_message>
<xml_diff>
--- a/Document/document_Hoc/tổng hợp tài liệu.xlsx
+++ b/Document/document_Hoc/tổng hợp tài liệu.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -18,6 +18,56 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>TÊN</t>
+  </si>
+  <si>
+    <t>use case</t>
+  </si>
+  <si>
+    <t>đặc tả</t>
+  </si>
+  <si>
+    <t>stackholder</t>
+  </si>
+  <si>
+    <t>yêu cầu kỹ thuật</t>
+  </si>
+  <si>
+    <t>thuật ngữ trong phần mềm</t>
+  </si>
+  <si>
+    <t>testcase</t>
+  </si>
+  <si>
+    <t>test plan</t>
+  </si>
+  <si>
+    <t>đánh giá rủi ro</t>
+  </si>
+  <si>
+    <t>quy trình nghiệp vụ</t>
+  </si>
+  <si>
+    <t>giới thiệu phần mềm</t>
+  </si>
+  <si>
+    <t>prototype</t>
+  </si>
+  <si>
+    <t>các phần lấy yêu cầu khách hàng</t>
+  </si>
+  <si>
+    <t>quản lý kế hoạch dự án</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
@@ -29,15 +79,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -45,12 +107,108 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,6 +302,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -179,6 +354,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -331,12 +523,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="26.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="5">
+        <v>13</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>